<commit_message>
Fixed problem with calculating r from model
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11002"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9D328606-0C31-C642-B185-BB907714C381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A7BB3C-8DC9-034E-B6B4-F899E546EA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="11820"/>
+    <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Species</t>
   </si>
@@ -111,15 +111,12 @@
   </si>
   <si>
     <t>Clavigralla tomentosicollis Nigeria</t>
-  </si>
-  <si>
-    <t>In model, r calculated using final 2 years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -959,11 +956,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,12 +1016,6 @@
       <c r="F2" s="1">
         <v>0.08</v>
       </c>
-      <c r="G2">
-        <v>5.9199999999999997E-4</v>
-      </c>
-      <c r="H2">
-        <v>4.9700000000000005E-4</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1046,13 +1037,10 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="G3">
-        <v>3.2799999999999999E-3</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="H3">
-        <v>1.1100000000000001E-3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
+        <v>2.75E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1074,12 +1062,7 @@
       <c r="F4" s="1">
         <v>0.06</v>
       </c>
-      <c r="G4">
-        <v>-5.1999999999999998E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5.8E-4</v>
-      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Ran models for three Clavigralla populations
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A7BB3C-8DC9-034E-B6B4-F899E546EA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAED3742-B984-514B-9972-8C1016BECA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -601,7 +601,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,7 +960,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,6 +1016,12 @@
       <c r="F2" s="1">
         <v>0.08</v>
       </c>
+      <c r="G2">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="H2">
+        <v>3.0099999999999998E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1062,7 +1068,12 @@
       <c r="F4" s="1">
         <v>0.06</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="G4">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.6799999999999999E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Fit temperature parameters for all locations
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAED3742-B984-514B-9972-8C1016BECA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C769B090-F8E9-7B42-B9C2-28BD24657CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Species</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Clavigralla tomentosicollis Nigeria</t>
+  </si>
+  <si>
+    <t>No diurnal variation</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -601,7 +604,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,12 +963,14 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1016,11 +1021,8 @@
       <c r="F2" s="1">
         <v>0.08</v>
       </c>
-      <c r="G2">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="H2">
-        <v>3.0099999999999998E-2</v>
+      <c r="I2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1037,16 +1039,13 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>0.109</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="F3">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="G3">
-        <v>2.3199999999999998E-2</v>
-      </c>
-      <c r="H3">
-        <v>2.75E-2</v>
+        <v>0.153</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1062,17 +1061,15 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
-        <v>4.1000000000000002E-2</v>
+      <c r="E4" s="1">
+        <v>0.15</v>
       </c>
       <c r="F4" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="G4">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1.6799999999999999E-2</v>
+        <v>0.153</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1087,6 +1084,21 @@
       </c>
       <c r="D5" t="s">
         <v>11</v>
+      </c>
+      <c r="E5">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.214</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Calculated r using TPC for all insect species
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C769B090-F8E9-7B42-B9C2-28BD24657CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4945B26-780A-F04B-8969-F0FFCBC5D011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="1480" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Species</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Clavigralla tomentosicollis Nigeria</t>
-  </si>
-  <si>
-    <t>No diurnal variation</t>
   </si>
 </sst>
 </file>
@@ -963,7 +960,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,13 +1013,10 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>7.2999999999999995E-2</v>
+        <v>0.126</v>
       </c>
       <c r="F2" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1038,14 +1032,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>0.13600000000000001</v>
+      <c r="E3" s="1">
+        <v>0.15</v>
       </c>
       <c r="F3">
-        <v>0.153</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1062,15 +1053,12 @@
         <v>11</v>
       </c>
       <c r="E4" s="1">
-        <v>0.15</v>
+        <v>0.154</v>
       </c>
       <c r="F4" s="1">
-        <v>0.153</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1086,20 +1074,13 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="F5">
-        <v>0.214</v>
-      </c>
-      <c r="G5" s="2">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1114,6 +1095,12 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
+      <c r="E6">
+        <v>0.127</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1128,6 +1115,12 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="E7">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1142,6 +1135,12 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
+      <c r="E8">
+        <v>0.107</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4.7E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1156,6 +1155,12 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
+      <c r="E9" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1170,6 +1175,12 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
+      <c r="E10" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.114</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1184,6 +1195,12 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
+      <c r="E11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-6.7000000000000004E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1198,6 +1215,12 @@
       <c r="D12" t="s">
         <v>20</v>
       </c>
+      <c r="E12">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1212,6 +1235,12 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
+      <c r="E13" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1225,6 +1254,12 @@
       </c>
       <c r="D14" t="s">
         <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fit life history trait responses for 8 insects
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E12559-D550-854A-90E5-E4DF1B427130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E161F81-12EA-4E49-B186-468B4028D74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="500" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +447,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -610,10 +616,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -972,7 +980,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G10" sqref="G10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,10 +1146,10 @@
       <c r="F5" s="1">
         <v>0.2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>2.9899999999999999E-2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>2.4899999999999999E-2</v>
       </c>
       <c r="I5" s="1">
@@ -1320,10 +1328,10 @@
       <c r="F10" s="1">
         <v>0.114</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>1.78E-2</v>
       </c>
       <c r="I10" s="1">

</xml_diff>

<commit_message>
Set all future climate data to start on 1/1/2025 and update temperature fits for all locations
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E161F81-12EA-4E49-B186-468B4028D74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338527B-F540-9245-90B2-BAD065371E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>Species</t>
   </si>
@@ -123,6 +123,72 @@
   </si>
   <si>
     <t>delta.model</t>
+  </si>
+  <si>
+    <r>
+      <t>Macrosiphum euphorbiae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Canada</t>
+    </r>
+  </si>
+  <si>
+    <t>Myzus persicae Canada</t>
+  </si>
+  <si>
+    <t>Subtropical</t>
+  </si>
+  <si>
+    <t>Toxoptera citricidus on C. unshiu Japan Chiba</t>
+  </si>
+  <si>
+    <t>Toxoptera citricidus on C. aurantium Japan Chiba</t>
+  </si>
+  <si>
+    <t>Aphis citricola Japan Chiba</t>
+  </si>
+  <si>
+    <t>Acyrthosiphon pisum UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>Bemisia argentifollii US Homestead</t>
+  </si>
+  <si>
+    <t>Rhopalosiphum rufiabdominalis US Naples</t>
+  </si>
+  <si>
+    <t>Aphis nasturtii US Weston</t>
+  </si>
+  <si>
+    <t>Diaphorina citri US Pompano Beach</t>
+  </si>
+  <si>
+    <t>Eriosoma lanigerum Australia Yathroo</t>
+  </si>
+  <si>
+    <t>Hyperomyzus lactucae Australia Acton</t>
+  </si>
+  <si>
+    <t>Aphis gossypii China Henan</t>
+  </si>
+  <si>
+    <t>Aulacorthum solani US Ithaca</t>
+  </si>
+  <si>
+    <t>Brevicoryne brassicae US Columbia</t>
+  </si>
+  <si>
+    <t>Myzus persicae US Columbia</t>
+  </si>
+  <si>
+    <t>Hyadaphis pseudobrassicae US Columbia</t>
   </si>
 </sst>
 </file>
@@ -133,7 +199,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +333,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -616,12 +688,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -977,15 +1050,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="1" max="1" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1488,6 +1561,244 @@
         <v>28</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>54.02</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>25.47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>26.14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>26.14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>26.24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23">
+        <v>30.9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>42.81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>42.81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>35.270000000000003</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>36.07</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>42.42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>38.93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>38.93</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>38.93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Calculated r for TPC and model
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68318D4B-153E-B24D-BB23-5B07A531C772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B482CF0-611B-ED4B-8389-29889394104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
     <t>Species</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Macrosiphum euphorbiae Canada</t>
+  </si>
+  <si>
+    <t>Including overwintering; extinct in model</t>
   </si>
 </sst>
 </file>
@@ -326,7 +329,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,12 +507,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -677,9 +674,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1037,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,21 +1097,21 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="F2" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G2">
         <v>4.58E-2</v>
       </c>
       <c r="H2">
-        <v>3.6200000000000003E-2</v>
+        <v>3.09E-2</v>
       </c>
       <c r="I2" s="1">
-        <f>(F2-E2)/E2</f>
-        <v>-9.9009900990099098E-2</v>
+        <f>MAX((F2-E2)/E2,-1)</f>
+        <v>-0.25742574257425749</v>
       </c>
       <c r="J2" s="1">
         <f>(H2-G2)/G2</f>
-        <v>-0.20960698689956325</v>
+        <v>-0.32532751091703055</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1140,15 +1137,15 @@
         <v>2.6599999999999999E-2</v>
       </c>
       <c r="H3">
-        <v>3.1300000000000001E-2</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I14" si="0">(F3-E3)/E3</f>
+        <f t="shared" ref="I3:I30" si="0">MAX((F3-E3)/E3,-1)</f>
         <v>0.67777777777777781</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J14" si="1">(H3-G3)/G3</f>
-        <v>0.17669172932330837</v>
+        <f t="shared" ref="J3:J18" si="1">(H3-G3)/G3</f>
+        <v>0.17293233082706769</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1171,10 +1168,10 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="G4">
-        <v>2.7400000000000001E-2</v>
+        <v>2.7300000000000001E-2</v>
       </c>
       <c r="H4" s="2">
-        <v>2.86E-2</v>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
@@ -1182,7 +1179,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>4.3795620437956193E-2</v>
+        <v>1.8315018315018205E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1199,24 +1196,24 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>3.4000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2.9899999999999999E-2</v>
-      </c>
-      <c r="H5" s="3">
-        <v>2.4899999999999999E-2</v>
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.23E-2</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>4.8823529411764701</v>
+        <v>1.5833333333333335</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>-0.16722408026755856</v>
+        <v>-0.25913621262458464</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1232,25 +1229,25 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6">
-        <v>7.6999999999999999E-2</v>
+      <c r="E6" s="1">
+        <v>0.10199999999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G6">
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="H6">
-        <v>4.3E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>-0.27272727272727271</v>
+        <v>-0.52941176470588236</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>-0.1224489795918367</v>
+        <v>-0.14285714285714288</v>
       </c>
       <c r="K6" t="s">
         <v>28</v>
@@ -1269,25 +1266,25 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7">
-        <v>5.8999999999999997E-2</v>
+      <c r="E7" s="1">
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>5.5E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G7">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="H7">
-        <v>5.7999999999999996E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>-6.779661016949147E-2</v>
+        <v>8.1632653061224414E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>-1.6949152542372926E-2</v>
+        <v>-5.0847457627118633E-2</v>
       </c>
       <c r="K7" t="s">
         <v>28</v>
@@ -1307,24 +1304,24 @@
         <v>11</v>
       </c>
       <c r="E8">
-        <v>7.6999999999999999E-2</v>
+        <v>0.104</v>
       </c>
       <c r="F8" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="G8">
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="H8">
-        <v>6.1999999999999998E-3</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>-2.5974025974025997E-2</v>
+        <v>-2.884615384615374E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>0.26530612244897961</v>
+        <v>0.20408163265306123</v>
       </c>
       <c r="K8" t="s">
         <v>28</v>
@@ -1344,24 +1341,24 @@
         <v>11</v>
       </c>
       <c r="E9" s="1">
-        <v>5.8999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F9" s="1">
-        <v>5.2999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G9">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="H9">
-        <v>5.7000000000000002E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.10169491525423727</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>3.6363636363636459E-2</v>
+        <v>-1.8181818181818073E-2</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
@@ -1381,24 +1378,24 @@
         <v>20</v>
       </c>
       <c r="E10" s="1">
-        <v>0.183</v>
+        <v>0.188</v>
       </c>
       <c r="F10" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="H10" s="4">
-        <v>1.78E-2</v>
+        <v>0.193</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>-0.37704918032786883</v>
+        <v>2.6595744680851088E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>7.8787878787878726E-2</v>
+        <v>1.3888888888888805E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1414,21 +1411,21 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11">
-        <v>0.18099999999999999</v>
+      <c r="E11" s="1">
+        <v>0.18</v>
       </c>
       <c r="F11" s="1">
-        <v>-6.6000000000000003E-2</v>
+        <v>0.155</v>
       </c>
       <c r="G11" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>-1.3646408839779005</v>
+        <v>-0.13888888888888887</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
@@ -1452,24 +1449,24 @@
         <v>20</v>
       </c>
       <c r="E12">
-        <v>0.17799999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F12" s="1">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="G12">
-        <v>2.4299999999999999E-2</v>
+        <v>0.153</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H12">
-        <v>2.87E-2</v>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.8764044943820225</v>
+        <v>-0.12068965517241374</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>0.18106995884773669</v>
+        <v>0.11199999999999988</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1489,21 +1486,21 @@
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>0.03</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G13" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H13">
-        <v>4.4999999999999997E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>-0.50819672131147542</v>
+        <v>-0.60655737704918034</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="1"/>
-        <v>-0.43750000000000006</v>
+        <v>-0.48749999999999999</v>
       </c>
       <c r="K13" t="s">
         <v>28</v>
@@ -1526,21 +1523,21 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>-0.01</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="G14">
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="H14">
-        <v>4.7999999999999996E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>-1.1694915254237288</v>
+        <v>-1</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="1"/>
-        <v>-0.42168674698795189</v>
+        <v>-0.46987951807228912</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
@@ -1559,6 +1556,29 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
+      <c r="E15" s="1">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.189</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H15">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.19574468085106378</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1573,9 +1593,32 @@
       <c r="D16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="E16" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.216</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.3E-3</v>
+      </c>
+      <c r="H16">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48484848484848481</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B17">
@@ -1587,9 +1630,32 @@
       <c r="D17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="E17" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.154</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="H17">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333338</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.365482233502538</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B18">
@@ -1601,9 +1667,32 @@
       <c r="D18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="E18" s="1">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="H18">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.295336787564768E-2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B19">
@@ -1615,9 +1704,32 @@
       <c r="D19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="E19" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.315</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.37E-2</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.6956521739130363E-2</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" ref="J19:J30" si="2">(H19-G19)/G19</f>
+        <v>-0.23888888888888882</v>
+      </c>
+      <c r="K19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B20">
@@ -1629,9 +1741,32 @@
       <c r="D20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="E20" s="1">
+        <v>0.247</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.46E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5020242914979838E-2</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="2"/>
+        <v>-4.1095890410958895E-2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B21">
@@ -1643,9 +1778,32 @@
       <c r="D21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="E21" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="H21">
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.75824175824175832</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1086309523809524</v>
+      </c>
+      <c r="K21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B22">
@@ -1657,8 +1815,31 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.40163934426229508</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="2"/>
+        <v>-7.9207920792079251E-2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1671,8 +1852,31 @@
       <c r="D23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2.35</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.45099999999999996</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1685,9 +1889,32 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="E24" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>7.06</v>
+      </c>
+      <c r="H24">
+        <v>6.33</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.48383233532934128</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.10339943342776198</v>
+      </c>
+      <c r="K24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B25">
@@ -1699,9 +1926,32 @@
       <c r="D25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="E25" s="1">
+        <v>0.222</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G25" s="2">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="H25">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.3063063063063113E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.37500000000000017</v>
+      </c>
+      <c r="K25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B26">
@@ -1713,9 +1963,32 @@
       <c r="D26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="E26" s="1">
+        <v>0.221</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="H26">
+        <v>5.3E-3</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.2398190045248931E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="2"/>
+        <v>8.1632653061224525E-2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B27">
@@ -1727,9 +2000,32 @@
       <c r="D27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="E27" s="1">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="H27">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.8529411764705882</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.1276595744680906E-2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B28">
@@ -1741,9 +2037,32 @@
       <c r="D28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="E28" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-0.248</v>
+      </c>
+      <c r="G28" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H28">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.14285714285714293</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B29">
@@ -1755,9 +2074,32 @@
       <c r="D29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="E29" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-0.26600000000000001</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H29">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.27272727272727265</v>
+      </c>
+      <c r="K29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B30">
@@ -1768,6 +2110,29 @@
       </c>
       <c r="D30" t="s">
         <v>20</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.38421052631578945</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="K30" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved calculation of r from DDE model
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B482CF0-611B-ED4B-8389-29889394104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7272CBBB-79F7-CD4E-A84F-157478B3CB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>Species</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Clavigralla tomentosicollis Nigeria</t>
-  </si>
-  <si>
-    <t>Extinct in future</t>
   </si>
   <si>
     <t>Including overwintering</t>
@@ -329,7 +326,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +504,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -670,13 +673,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1034,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,10 +1079,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1110,7 +1118,7 @@
         <v>-0.25742574257425749</v>
       </c>
       <c r="J2" s="1">
-        <f>(H2-G2)/G2</f>
+        <f>MAX((H2-G2)/G2,-1)</f>
         <v>-0.32532751091703055</v>
       </c>
     </row>
@@ -1144,7 +1152,7 @@
         <v>0.67777777777777781</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J18" si="1">(H3-G3)/G3</f>
+        <f t="shared" ref="J3:J30" si="1">MAX((H3-G3)/G3,-1)</f>
         <v>0.17293233082706769</v>
       </c>
     </row>
@@ -1165,21 +1173,21 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>0.13900000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G4">
-        <v>2.7300000000000001E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.7799999999999998E-2</v>
+        <v>1.52</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1.76</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>0.57954545454545481</v>
+        <v>0.55681818181818199</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>1.8315018315018205E-2</v>
+        <v>0.15789473684210525</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1250,7 +1258,7 @@
         <v>-0.14285714285714288</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1287,7 +1295,7 @@
         <v>-5.0847457627118633E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1324,7 +1332,7 @@
         <v>0.20408163265306123</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1361,7 +1369,7 @@
         <v>-1.8181818181818073E-2</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1411,28 +1419,25 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="10">
         <v>0.18</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="10">
         <v>0.155</v>
       </c>
-      <c r="G11" s="2">
-        <v>1.6799999999999999E-2</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="G11" s="4">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="I11" s="10">
         <f t="shared" si="0"/>
         <v>-0.13888888888888887</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
+        <v>8.3102493074792325E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1503,7 +1508,7 @@
         <v>-0.48749999999999999</v>
       </c>
       <c r="K13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1540,18 +1545,18 @@
         <v>-0.46987951807228912</v>
       </c>
       <c r="K14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>35.380000000000003</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
@@ -1577,18 +1582,18 @@
         <v>0.34</v>
       </c>
       <c r="K15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>35.380000000000003</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1614,12 +1619,12 @@
         <v>0.48484848484848481</v>
       </c>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>54.02</v>
@@ -1651,18 +1656,18 @@
         <v>-0.365482233502538</v>
       </c>
       <c r="K17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>25.47</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1688,18 +1693,18 @@
         <v>1.295336787564768E-2</v>
       </c>
       <c r="K18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>26.14</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -1721,22 +1726,22 @@
         <v>-8.6956521739130363E-2</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" ref="J19:J30" si="2">(H19-G19)/G19</f>
+        <f t="shared" si="1"/>
         <v>-0.23888888888888882</v>
       </c>
       <c r="K19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>26.14</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -1758,22 +1763,22 @@
         <v>8.5020242914979838E-2</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.1095890410958895E-2</v>
       </c>
       <c r="K20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>26.24</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -1795,22 +1800,22 @@
         <v>-0.75824175824175832</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.1086309523809524</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>30.9</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -1832,16 +1837,16 @@
         <v>-0.40163934426229508</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-7.9207920792079251E-2</v>
       </c>
       <c r="K22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>42.81</v>
@@ -1852,33 +1857,33 @@
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="G23" s="2">
-        <v>2.35</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.45099999999999996</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="2"/>
+      <c r="E23" s="7">
+        <v>0.188</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.496</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H23" s="9">
+        <v>-2.3E-2</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6382978723404256</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="K23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>42.81</v>
@@ -1906,22 +1911,22 @@
         <v>-0.48383233532934128</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.10339943342776198</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>35.270000000000003</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
@@ -1943,16 +1948,16 @@
         <v>-6.3063063063063113E-2</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.37500000000000017</v>
       </c>
       <c r="K25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>36.07</v>
@@ -1980,16 +1985,16 @@
         <v>-7.2398190045248931E-2</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.1632653061224525E-2</v>
       </c>
       <c r="K26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>42.42</v>
@@ -2017,16 +2022,16 @@
         <v>-0.8529411764705882</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-2.1276595744680906E-2</v>
       </c>
       <c r="K27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>38.93</v>
@@ -2054,16 +2059,16 @@
         <v>-1</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.14285714285714293</v>
       </c>
       <c r="K28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>38.93</v>
@@ -2091,16 +2096,16 @@
         <v>-1</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.27272727272727265</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>38.93</v>
@@ -2128,11 +2133,11 @@
         <v>-0.38421052631578945</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.33333333333333331</v>
       </c>
       <c r="K30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>